<commit_message>
add merged jsa data file
</commit_message>
<xml_diff>
--- a/workbook_for_class.xlsx
+++ b/workbook_for_class.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="17955" windowHeight="12045"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="17955" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Main_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot_Table_and_Chart" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main_Data!$A$1:$P$79</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId5"/>
+  </pivotCaches>
 </workbook>
 </file>
 
@@ -82,8 +86,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -107,12 +119,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,6 +258,1994 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[workbook_for_class.xlsx]Pivot_Table_and_Chart!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="151251200"/>
+        <c:axId val="151252992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="151251200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151252992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="151252992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151251200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jon Minton" refreshedDate="41941.487670254632" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="78">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:P79" sheet="Main_Data"/>
+  </cacheSource>
+  <cacheFields count="16">
+    <cacheField name="year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1980" maxValue="2005" count="26">
+        <n v="1980"/>
+        <n v="1981"/>
+        <n v="1982"/>
+        <n v="1983"/>
+        <n v="1984"/>
+        <n v="1985"/>
+        <n v="1986"/>
+        <n v="1987"/>
+        <n v="1988"/>
+        <n v="1989"/>
+        <n v="1990"/>
+        <n v="1991"/>
+        <n v="1992"/>
+        <n v="1993"/>
+        <n v="1994"/>
+        <n v="1995"/>
+        <n v="1996"/>
+        <n v="1997"/>
+        <n v="1998"/>
+        <n v="1999"/>
+        <n v="2000"/>
+        <n v="2001"/>
+        <n v="2002"/>
+        <n v="2003"/>
+        <n v="2004"/>
+        <n v="2005"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="area" numFmtId="0">
+      <sharedItems count="3">
+        <s v="scotland"/>
+        <s v="east_end"/>
+        <s v="west_end"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="all_tenant_sales" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="32679"/>
+    </cacheField>
+    <cacheField name="flat_tenant_sales" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="12184"/>
+    </cacheField>
+    <cacheField name="house_tenant_sales" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="21378"/>
+    </cacheField>
+    <cacheField name="house_price_lower_quartile" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="26500" maxValue="145000" count="39">
+        <m/>
+        <n v="36000"/>
+        <n v="37000"/>
+        <n v="37250"/>
+        <n v="38000"/>
+        <n v="38400"/>
+        <n v="39000"/>
+        <n v="40000"/>
+        <n v="41500"/>
+        <n v="43000"/>
+        <n v="46500"/>
+        <n v="55000"/>
+        <n v="67000"/>
+        <n v="77250"/>
+        <n v="26875"/>
+        <n v="26500"/>
+        <n v="28000"/>
+        <n v="27500"/>
+        <n v="27000"/>
+        <n v="27750"/>
+        <n v="28998"/>
+        <n v="28500"/>
+        <n v="29950"/>
+        <n v="32000"/>
+        <n v="41950"/>
+        <n v="54200"/>
+        <n v="42000"/>
+        <n v="44700"/>
+        <n v="46000"/>
+        <n v="46600"/>
+        <n v="52000"/>
+        <n v="60000"/>
+        <n v="61516"/>
+        <n v="74950"/>
+        <n v="77950"/>
+        <n v="93500"/>
+        <n v="118500"/>
+        <n v="139500"/>
+        <n v="145000"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="house_price_mean" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="30000" maxValue="185620" count="40">
+        <m/>
+        <n v="46044"/>
+        <n v="48000"/>
+        <n v="48500"/>
+        <n v="49025"/>
+        <n v="50500"/>
+        <n v="51953"/>
+        <n v="54000"/>
+        <n v="56448"/>
+        <n v="59460"/>
+        <n v="65927"/>
+        <n v="77511"/>
+        <n v="94292"/>
+        <n v="107910"/>
+        <n v="30000"/>
+        <n v="30500"/>
+        <n v="35454"/>
+        <n v="32250"/>
+        <n v="33299"/>
+        <n v="30377"/>
+        <n v="32382"/>
+        <n v="33650"/>
+        <n v="34263"/>
+        <n v="36700"/>
+        <n v="43837"/>
+        <n v="56620"/>
+        <n v="63000"/>
+        <n v="50261"/>
+        <n v="55357"/>
+        <n v="56341"/>
+        <n v="58794"/>
+        <n v="64726"/>
+        <n v="75691"/>
+        <n v="82119"/>
+        <n v="94798"/>
+        <n v="106169"/>
+        <n v="124395"/>
+        <n v="151360"/>
+        <n v="181978"/>
+        <n v="185620"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="house_price_median" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="29500" maxValue="176500"/>
+    </cacheField>
+    <cacheField name="house_price_upper_quartile" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="30000" maxValue="213250"/>
+    </cacheField>
+    <cacheField name="number_of_house_sales" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="189" maxValue="114125"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_16_to_24" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="233" maxValue="130076"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_25_to_49" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="281" maxValue="150329"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_50_plus" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="207" maxValue="96286"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_female" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="234" maxValue="117434"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_male" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="377" maxValue="162329"/>
+    </cacheField>
+    <cacheField name="jsa_claimants_total" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="475" maxValue="215064"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="78">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4774"/>
+    <n v="595"/>
+    <n v="4179"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8740"/>
+    <n v="1015"/>
+    <n v="7725"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="12219"/>
+    <n v="1641"/>
+    <n v="10578"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="14986"/>
+    <n v="2068"/>
+    <n v="12918"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="13761"/>
+    <n v="1815"/>
+    <n v="11946"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="12520"/>
+    <n v="1960"/>
+    <n v="10560"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="11858"/>
+    <n v="1968"/>
+    <n v="9890"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="15896"/>
+    <n v="4069"/>
+    <n v="11827"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="24922"/>
+    <n v="7706"/>
+    <n v="17216"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="32679"/>
+    <n v="11301"/>
+    <n v="21378"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="29040"/>
+    <n v="12184"/>
+    <n v="16856"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="20167"/>
+    <n v="8433"/>
+    <n v="11734"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="0"/>
+    <n v="20896"/>
+    <n v="8242"/>
+    <n v="12654"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="0"/>
+    <n v="17556"/>
+    <n v="6578"/>
+    <n v="10978"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="42750"/>
+    <m/>
+    <n v="79300"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="0"/>
+    <n v="18907"/>
+    <n v="6860"/>
+    <n v="12047"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="44625"/>
+    <m/>
+    <n v="79661"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+    <n v="14747"/>
+    <n v="5452"/>
+    <n v="9295"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="44825"/>
+    <n v="55750"/>
+    <n v="77489"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="0"/>
+    <n v="11271"/>
+    <n v="3987"/>
+    <n v="7284"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="45500"/>
+    <m/>
+    <n v="75361"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="0"/>
+    <n v="15514"/>
+    <n v="5604"/>
+    <n v="9910"/>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="46500"/>
+    <n v="58500"/>
+    <n v="78289"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="0"/>
+    <n v="13559"/>
+    <n v="5297"/>
+    <n v="8262"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="48000"/>
+    <n v="60000"/>
+    <n v="82959"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="0"/>
+    <n v="12870"/>
+    <n v="4680"/>
+    <n v="8190"/>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="50000"/>
+    <n v="62500"/>
+    <n v="87363"/>
+    <n v="65638"/>
+    <n v="74880"/>
+    <n v="47865"/>
+    <n v="60004"/>
+    <n v="89317"/>
+    <n v="126554"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="0"/>
+    <n v="13613"/>
+    <n v="4890"/>
+    <n v="8723"/>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="52000"/>
+    <n v="65995"/>
+    <n v="91517"/>
+    <n v="127983"/>
+    <n v="147713"/>
+    <n v="96286"/>
+    <n v="109151"/>
+    <n v="157872"/>
+    <n v="215064"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="0"/>
+    <n v="12946"/>
+    <n v="4780"/>
+    <n v="8166"/>
+    <x v="9"/>
+    <x v="9"/>
+    <n v="54650"/>
+    <n v="69950"/>
+    <n v="97656"/>
+    <n v="130076"/>
+    <n v="146807"/>
+    <n v="94328"/>
+    <n v="117434"/>
+    <n v="162329"/>
+    <n v="192501"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="0"/>
+    <n v="15762"/>
+    <n v="5621"/>
+    <n v="10141"/>
+    <x v="10"/>
+    <x v="10"/>
+    <n v="59500"/>
+    <n v="77500"/>
+    <n v="108817"/>
+    <n v="118627"/>
+    <n v="147641"/>
+    <n v="80149"/>
+    <n v="106225"/>
+    <n v="160138"/>
+    <n v="182068"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="0"/>
+    <n v="17455"/>
+    <n v="6242"/>
+    <n v="11213"/>
+    <x v="11"/>
+    <x v="11"/>
+    <n v="70000"/>
+    <n v="91500"/>
+    <n v="107725"/>
+    <n v="126908"/>
+    <n v="150329"/>
+    <n v="88440"/>
+    <n v="109366"/>
+    <n v="153420"/>
+    <n v="162706"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="0"/>
+    <n v="12682"/>
+    <n v="4896"/>
+    <n v="7786"/>
+    <x v="12"/>
+    <x v="12"/>
+    <n v="86000"/>
+    <n v="113000"/>
+    <n v="99009"/>
+    <n v="121578"/>
+    <n v="149027"/>
+    <n v="85029"/>
+    <n v="95868"/>
+    <n v="149932"/>
+    <n v="153173"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="0"/>
+    <n v="10784"/>
+    <n v="4419"/>
+    <n v="6365"/>
+    <x v="13"/>
+    <x v="13"/>
+    <n v="97000"/>
+    <n v="128000"/>
+    <n v="114125"/>
+    <n v="118296"/>
+    <n v="146987"/>
+    <n v="71819"/>
+    <n v="101042"/>
+    <n v="149788"/>
+    <n v="154897"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="11"/>
+    <n v="11"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="27"/>
+    <n v="23"/>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="50"/>
+    <n v="43"/>
+    <n v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="22"/>
+    <n v="20"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="1"/>
+    <n v="35"/>
+    <n v="33"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="1"/>
+    <n v="27"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="14"/>
+    <x v="14"/>
+    <n v="30000"/>
+    <n v="30000"/>
+    <n v="218"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="1"/>
+    <n v="23"/>
+    <n v="21"/>
+    <n v="2"/>
+    <x v="15"/>
+    <x v="15"/>
+    <n v="30000"/>
+    <n v="30500"/>
+    <n v="208"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+    <n v="17"/>
+    <n v="17"/>
+    <n v="0"/>
+    <x v="16"/>
+    <x v="16"/>
+    <n v="32998"/>
+    <n v="37950"/>
+    <n v="215"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="1"/>
+    <n v="12"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="17"/>
+    <x v="17"/>
+    <n v="30000"/>
+    <n v="35000"/>
+    <n v="246"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="1"/>
+    <n v="20"/>
+    <n v="19"/>
+    <n v="1"/>
+    <x v="18"/>
+    <x v="18"/>
+    <n v="32750"/>
+    <n v="35925"/>
+    <n v="206"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="1"/>
+    <n v="11"/>
+    <n v="10"/>
+    <n v="1"/>
+    <x v="19"/>
+    <x v="19"/>
+    <n v="29500"/>
+    <n v="34000"/>
+    <n v="189"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="1"/>
+    <n v="15"/>
+    <n v="14"/>
+    <n v="1"/>
+    <x v="20"/>
+    <x v="20"/>
+    <n v="31000"/>
+    <n v="35000"/>
+    <n v="305"/>
+    <n v="233"/>
+    <n v="343"/>
+    <n v="211"/>
+    <n v="234"/>
+    <n v="533"/>
+    <n v="813"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="1"/>
+    <n v="22"/>
+    <n v="17"/>
+    <n v="5"/>
+    <x v="17"/>
+    <x v="21"/>
+    <n v="30500"/>
+    <n v="37975"/>
+    <n v="340"/>
+    <n v="487"/>
+    <n v="607"/>
+    <n v="455"/>
+    <n v="447"/>
+    <n v="888"/>
+    <n v="1369"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="1"/>
+    <n v="15"/>
+    <n v="14"/>
+    <n v="1"/>
+    <x v="21"/>
+    <x v="22"/>
+    <n v="33950"/>
+    <n v="39500"/>
+    <n v="284"/>
+    <n v="515"/>
+    <n v="520"/>
+    <n v="513"/>
+    <n v="561"/>
+    <n v="817"/>
+    <n v="1122"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="1"/>
+    <n v="26"/>
+    <n v="24"/>
+    <n v="2"/>
+    <x v="22"/>
+    <x v="23"/>
+    <n v="35250"/>
+    <n v="44875"/>
+    <n v="394"/>
+    <n v="486"/>
+    <n v="496"/>
+    <n v="413"/>
+    <n v="502"/>
+    <n v="729"/>
+    <n v="998"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="1"/>
+    <n v="15"/>
+    <n v="14"/>
+    <n v="1"/>
+    <x v="23"/>
+    <x v="24"/>
+    <n v="43000"/>
+    <n v="52000"/>
+    <n v="504"/>
+    <n v="535"/>
+    <n v="467"/>
+    <n v="401"/>
+    <n v="496"/>
+    <n v="676"/>
+    <n v="871"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="1"/>
+    <n v="13"/>
+    <n v="11"/>
+    <n v="2"/>
+    <x v="24"/>
+    <x v="25"/>
+    <n v="50402"/>
+    <n v="64100"/>
+    <n v="489"/>
+    <n v="560"/>
+    <n v="461"/>
+    <n v="377"/>
+    <n v="508"/>
+    <n v="560"/>
+    <n v="709"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="1"/>
+    <n v="17"/>
+    <n v="14"/>
+    <n v="3"/>
+    <x v="25"/>
+    <x v="26"/>
+    <n v="63000"/>
+    <n v="68500"/>
+    <n v="517"/>
+    <n v="566"/>
+    <n v="470"/>
+    <n v="308"/>
+    <n v="527"/>
+    <n v="531"/>
+    <n v="658"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="7"/>
+    <n v="3"/>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="17"/>
+    <n v="14"/>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <n v="11"/>
+    <n v="11"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <n v="13"/>
+    <n v="12"/>
+    <n v="1"/>
+    <x v="26"/>
+    <x v="27"/>
+    <n v="50500"/>
+    <n v="57200"/>
+    <n v="681"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <x v="27"/>
+    <x v="28"/>
+    <n v="53000"/>
+    <n v="60000"/>
+    <n v="694"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="0"/>
+    <x v="28"/>
+    <x v="29"/>
+    <n v="56900"/>
+    <n v="65000"/>
+    <n v="578"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+    <x v="29"/>
+    <x v="30"/>
+    <n v="58000"/>
+    <n v="65250"/>
+    <n v="674"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="2"/>
+    <n v="17"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="30"/>
+    <x v="31"/>
+    <n v="62500"/>
+    <n v="77000"/>
+    <n v="634"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="2"/>
+    <n v="14"/>
+    <n v="14"/>
+    <n v="0"/>
+    <x v="31"/>
+    <x v="32"/>
+    <n v="73500"/>
+    <n v="88000"/>
+    <n v="685"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <x v="32"/>
+    <x v="33"/>
+    <n v="80000"/>
+    <n v="98250"/>
+    <n v="647"/>
+    <n v="256"/>
+    <n v="281"/>
+    <n v="207"/>
+    <n v="235"/>
+    <n v="377"/>
+    <n v="669"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="2"/>
+    <n v="15"/>
+    <n v="12"/>
+    <n v="3"/>
+    <x v="33"/>
+    <x v="34"/>
+    <n v="87000"/>
+    <n v="112875"/>
+    <n v="656"/>
+    <n v="526"/>
+    <n v="475"/>
+    <n v="420"/>
+    <n v="464"/>
+    <n v="597"/>
+    <n v="1054"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="2"/>
+    <n v="18"/>
+    <n v="18"/>
+    <n v="0"/>
+    <x v="34"/>
+    <x v="35"/>
+    <n v="95054"/>
+    <n v="130000"/>
+    <n v="715"/>
+    <n v="619"/>
+    <n v="410"/>
+    <n v="397"/>
+    <n v="587"/>
+    <n v="559"/>
+    <n v="835"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="2"/>
+    <n v="20"/>
+    <n v="19"/>
+    <n v="1"/>
+    <x v="35"/>
+    <x v="36"/>
+    <n v="126000"/>
+    <n v="143400"/>
+    <n v="707"/>
+    <n v="480"/>
+    <n v="482"/>
+    <n v="351"/>
+    <n v="506"/>
+    <n v="552"/>
+    <n v="775"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="2"/>
+    <n v="9"/>
+    <n v="9"/>
+    <n v="0"/>
+    <x v="36"/>
+    <x v="37"/>
+    <n v="147000"/>
+    <n v="170000"/>
+    <n v="854"/>
+    <n v="596"/>
+    <n v="473"/>
+    <n v="387"/>
+    <n v="541"/>
+    <n v="456"/>
+    <n v="612"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="2"/>
+    <n v="11"/>
+    <n v="11"/>
+    <n v="0"/>
+    <x v="37"/>
+    <x v="38"/>
+    <n v="176500"/>
+    <n v="206000"/>
+    <n v="677"/>
+    <n v="629"/>
+    <n v="481"/>
+    <n v="379"/>
+    <n v="527"/>
+    <n v="447"/>
+    <n v="517"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <x v="38"/>
+    <x v="39"/>
+    <n v="175000"/>
+    <n v="213250"/>
+    <n v="722"/>
+    <n v="580"/>
+    <n v="530"/>
+    <n v="364"/>
+    <n v="580"/>
+    <n v="416"/>
+    <n v="475"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0">
+      <items count="27">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="40">
+        <item x="15"/>
+        <item x="14"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="16"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="24"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="10"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="25"/>
+        <item x="11"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="12"/>
+        <item x="33"/>
+        <item x="13"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="41">
+        <item x="14"/>
+        <item x="19"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="20"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="16"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="27"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="8"/>
+        <item x="25"/>
+        <item x="30"/>
+        <item x="9"/>
+        <item x="26"/>
+        <item x="31"/>
+        <item x="10"/>
+        <item x="32"/>
+        <item x="11"/>
+        <item x="33"/>
+        <item x="12"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="13"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,53 +2558,53 @@
     <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2775,13 +4896,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2795,4 +5022,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>